<commit_message>
updated CSV exporter to include 'normal' cells in tthe csv - this required adding some extra accessor methods to cell and sheets to get the cells with contents, and get the sheet name and index directly from a cell
</commit_message>
<xml_diff>
--- a/src/test/resources/simple_annotated_book.xlsx
+++ b/src/test/resources/simple_annotated_book.xlsx
@@ -1,30 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
-  <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19680" windowHeight="15200" tabRatio="199"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="199"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet0" sheetId="1" r:id="rId1"/>
     <sheet name="HiddenSheet" sheetId="2" state="hidden" r:id="rId2"/>
     <sheet name="wksowlv0" sheetId="3" state="veryHidden" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="wksowlv0">wksowlv0!$B$4:$B$10</definedName>
   </definedNames>
-  <calcPr calcId="101716" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>ExperimentDesignType</t>
   </si>
@@ -90,6 +86,12 @@
   </si>
   <si>
     <t>TechnologicalDesign</t>
+  </si>
+  <si>
+    <t>Some content on sheet 2</t>
+  </si>
+  <si>
+    <t>Simple Annotated Book</t>
   </si>
 </sst>
 </file>
@@ -137,75 +139,12 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00DD0806"/>
-      <rgbColor rgb="001FB714"/>
-      <rgbColor rgb="000000D4"/>
-      <rgbColor rgb="00FCF305"/>
-      <rgbColor rgb="00F20884"/>
-      <rgbColor rgb="0000ABEA"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -354,16 +293,20 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
+                <a:shade val="51000"/>
                 <a:satMod val="130000"/>
               </a:schemeClr>
             </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -514,13 +457,11 @@
         </a:ln>
         <a:effectLst/>
         <a:extLst>
-          <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
+          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
             <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
-                <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="000000">
-                    <a:alpha val="74998"/>
-                  </a:srgbClr>
+                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="808080"/>
                 </a:outerShdw>
               </a:effectLst>
             </a14:hiddenEffects>
@@ -558,13 +499,11 @@
         </a:ln>
         <a:effectLst/>
         <a:extLst>
-          <a:ext uri="{AF507438-7753-43e0-B8FC-AC1667EBCBE1}">
+          <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
             <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
-                <a:outerShdw blurRad="63500" dist="38099" dir="2700000" algn="ctr" rotWithShape="0">
-                  <a:srgbClr val="000000">
-                    <a:alpha val="74998"/>
-                  </a:srgbClr>
+                <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
+                  <a:srgbClr val="808080"/>
                 </a:outerShdw>
               </a:effectLst>
             </a14:hiddenEffects>
@@ -581,13 +520,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D12:E12"/>
+  <dimension ref="B3:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="12" spans="4:5">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="D12" t="s">
         <v>1</v>
       </c>
@@ -604,15 +550,10 @@
   </dataValidations>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
+  <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -620,22 +561,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0527777777777778" bottom="1.0527777777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <headerFooter>
+  <headerFooter alignWithMargins="0">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -643,11 +579,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView showRuler="0" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -655,7 +591,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -666,7 +602,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -677,7 +613,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -685,7 +621,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -693,7 +629,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -701,7 +637,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>14</v>
       </c>
@@ -709,7 +645,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -717,7 +653,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -725,7 +661,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -736,10 +672,26 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="6" spans="5:5" x14ac:dyDescent="0.2">
+      <c r="E6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>